<commit_message>
Added ddt to registration
</commit_message>
<xml_diff>
--- a/src/test/resources/RegistrationData.xlsx
+++ b/src/test/resources/RegistrationData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mini Project\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\PSLMiniProject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C8914E-6DDB-43DA-B617-16ED66E813AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A548C30-F87E-41D5-8766-80821A381EC5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="21">
   <si>
     <t>Errol5</t>
   </si>
@@ -52,13 +52,49 @@
   </si>
   <si>
     <t>demo4@example.com</t>
+  </si>
+  <si>
+    <t>Raunak</t>
+  </si>
+  <si>
+    <t>Naik</t>
+  </si>
+  <si>
+    <t>testing@example.com</t>
+  </si>
+  <si>
+    <t>testing123</t>
+  </si>
+  <si>
+    <t>test4567</t>
+  </si>
+  <si>
+    <t>testing1@example.com</t>
+  </si>
+  <si>
+    <t>testing2@example.com</t>
+  </si>
+  <si>
+    <t>testing3@example.com</t>
+  </si>
+  <si>
+    <t>Raunakabcdefghijklmnopqrstuvwxyza</t>
+  </si>
+  <si>
+    <t>Naikabcdefghijklmnopqrstuvwxyzabc</t>
+  </si>
+  <si>
+    <t>testing4@example.com</t>
+  </si>
+  <si>
+    <t>testing5@example.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,6 +106,19 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -98,8 +147,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -381,25 +430,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="26.453125" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D1">
@@ -412,14 +463,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D2">
@@ -432,11 +483,11 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D3">
@@ -449,14 +500,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D4">
@@ -468,16 +519,16 @@
       <c r="F4" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D5" t="s">
@@ -490,18 +541,160 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2123434565</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2123434565</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2123434565</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="2">
+        <v>12</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2123434565</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2123434565</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="2">
+        <v>2.12343456521312E+35</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C1" r:id="rId1" xr:uid="{98EA15EE-30AE-4D63-9471-EAC6B9357D94}"/>
     <hyperlink ref="C2" r:id="rId2" xr:uid="{391D5505-CD6F-4EF8-BCB9-DDB17D38E9FA}"/>
     <hyperlink ref="C3" r:id="rId3" xr:uid="{10138BEA-23DD-449C-A35B-C618A68B75AE}"/>
     <hyperlink ref="C4" r:id="rId4" xr:uid="{5DB6AE30-4916-4133-A545-6730329B0289}"/>
     <hyperlink ref="C5" r:id="rId5" xr:uid="{8B2824A2-89A8-413E-80A8-D7D49B6886E3}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{DEC12846-F637-4262-B38C-0F660F53A106}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{EE29CEF4-BEA8-4F88-8AF3-689DDDC33F72}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{8BC92C34-F772-4EE5-A63C-F0AD276B46BF}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{DE62A795-4C1D-4994-9CCF-00B20CCA36F1}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{F65885B8-7303-4E24-89F4-9211AD7979A4}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{12ACB556-7E51-48FF-BAA2-BAEE75DA9EEF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Chnaged xpath to css path in Registration and contact us POM
</commit_message>
<xml_diff>
--- a/src/test/resources/RegistrationData.xlsx
+++ b/src/test/resources/RegistrationData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\PSLMiniProject\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maven Project\PSLMiniProject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A548C30-F87E-41D5-8766-80821A381EC5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CD441B-B134-4796-A920-8DC18ECA7CD1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="23">
   <si>
     <t>Errol5</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>testing5@example.com</t>
+  </si>
+  <si>
+    <t>22222222222222222222222222222222222</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -145,10 +151,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -433,17 +440,17 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.453125" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,7 +470,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -483,7 +490,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -500,7 +507,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -521,7 +528,7 @@
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -541,7 +548,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -561,7 +568,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -569,7 +576,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D7" s="2">
         <v>2123434565</v>
@@ -581,7 +588,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>10</v>
@@ -599,7 +606,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -609,8 +616,8 @@
       <c r="C9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="2">
-        <v>12</v>
+      <c r="D9" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>12</v>
@@ -619,7 +626,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -639,7 +646,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -659,7 +666,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -669,8 +676,8 @@
       <c r="C12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="2">
-        <v>2.12343456521312E+35</v>
+      <c r="D12" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Added comments for TC_OC_REG_002 and 003
</commit_message>
<xml_diff>
--- a/src/test/resources/RegistrationData.xlsx
+++ b/src/test/resources/RegistrationData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maven Project\PSLMiniProject\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diffa_pinto\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CD441B-B134-4796-A920-8DC18ECA7CD1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9172EE10-6F63-4DFE-93F1-5058A7D4A464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="25">
   <si>
     <t>Errol5</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>Diffa</t>
+  </si>
+  <si>
+    <t>P</t>
   </si>
 </sst>
 </file>
@@ -440,7 +446,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -472,16 +478,16 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D2">
-        <v>122345</v>
+        <v>2123434565</v>
       </c>
       <c r="E2">
         <v>123</v>
@@ -492,19 +498,19 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D3">
-        <v>123455</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>3</v>
+        <v>2123434565</v>
+      </c>
+      <c r="E3">
+        <v>12345678</v>
+      </c>
+      <c r="F3">
+        <v>12345678</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
modified login css test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/RegistrationData.xlsx
+++ b/src/test/resources/RegistrationData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maven Project\PSLMiniProject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CD441B-B134-4796-A920-8DC18ECA7CD1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A889EF6-619B-4603-8D49-35EC306BDE62}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Registration" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="29">
   <si>
     <t>Errol5</t>
   </si>
@@ -94,6 +95,24 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>tester1@gmail.com</t>
+  </si>
+  <si>
+    <t>test123</t>
+  </si>
+  <si>
+    <t>tester@gmail.com</t>
+  </si>
+  <si>
+    <t>tester123</t>
   </si>
 </sst>
 </file>
@@ -439,8 +458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -704,4 +723,86 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2F1686C-AD4C-4E50-BE6C-ECE2756B16FE}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
checkout pom not working
</commit_message>
<xml_diff>
--- a/src/test/resources/RegistrationData.xlsx
+++ b/src/test/resources/RegistrationData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maven Project\PSLMiniProject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D003D9E1-C02F-4E79-BE19-324C69A477C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{407C4D51-1A5F-404F-B681-A37056926937}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -727,10 +727,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2F1686C-AD4C-4E50-BE6C-ECE2756B16FE}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -770,20 +770,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-    </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -799,6 +791,14 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added SearchData.java and SearchData.xlsx
</commit_message>
<xml_diff>
--- a/src/test/resources/RegistrationData.xlsx
+++ b/src/test/resources/RegistrationData.xlsx
@@ -3,20 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maven Project\PSLMiniProject\src\test\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{407C4D51-1A5F-404F-B681-A37056926937}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{D6E93CC8-9D00-44E1-BC54-D83B74003192}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="19455" windowHeight="13890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:N17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -458,18 +454,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="26.453125" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -489,7 +485,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -509,7 +505,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -526,7 +522,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -547,7 +543,7 @@
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -567,7 +563,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -587,7 +583,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -595,7 +591,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D7" s="2">
         <v>2123434565</v>
@@ -607,7 +603,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>10</v>
@@ -625,7 +621,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -645,7 +641,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -665,7 +661,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -685,7 +681,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -729,16 +725,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2F1686C-AD4C-4E50-BE6C-ECE2756B16FE}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.453125" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -746,7 +742,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -754,7 +750,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -762,7 +758,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -770,7 +766,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -778,7 +774,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -786,7 +782,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -794,7 +790,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>

</xml_diff>